<commit_message>
New icon, plus some bug fixes
</commit_message>
<xml_diff>
--- a/Image dimensions.xlsx
+++ b/Image dimensions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\ToodleDo10Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Toodledo10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>H</t>
   </si>
@@ -372,7 +372,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,18 +424,18 @@
         <v>853.33333333333337</v>
       </c>
       <c r="E2" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F2" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G2" s="1">
         <f>B2/2-F2/2</f>
-        <v>403.5</v>
+        <v>347</v>
       </c>
       <c r="H2">
         <f>A2/2-E2/2</f>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -457,18 +457,18 @@
         <v>480</v>
       </c>
       <c r="E3" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F3" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G6" si="2">B3/2-F3/2</f>
-        <v>123.5</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H6" si="3">A3/2-E3/2</f>
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -490,18 +490,18 @@
         <v>853.33333333333337</v>
       </c>
       <c r="E4" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F4" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="2"/>
-        <v>403.5</v>
+        <v>347</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -523,18 +523,18 @@
         <v>512</v>
       </c>
       <c r="E5" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F5" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>147.5</v>
+        <v>91</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -556,21 +556,18 @@
         <v>480</v>
       </c>
       <c r="E6" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F6" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="2"/>
-        <v>123.5</v>
+        <v>67</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -589,21 +586,18 @@
         <v>790.66666666666663</v>
       </c>
       <c r="E7" s="1">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="F7" s="1">
-        <v>473</v>
+        <v>586</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ref="G7:G9" si="4">B7/2-F7/2</f>
-        <v>356.5</v>
+        <v>300</v>
       </c>
       <c r="H7">
         <f t="shared" ref="H7:H9" si="5">A7/2-E7/2</f>
-        <v>654</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,9 +629,6 @@
         <f t="shared" si="5"/>
         <v>294</v>
       </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -667,9 +658,6 @@
       <c r="H9">
         <f t="shared" si="5"/>
         <v>82</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
App name and logo change
</commit_message>
<xml_diff>
--- a/Image dimensions.xlsx
+++ b/Image dimensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>H</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Logo V</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -369,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +379,7 @@
     <col min="5" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>720</v>
       </c>
@@ -427,21 +424,18 @@
         <v>620</v>
       </c>
       <c r="F2" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G2" s="1">
         <f>B2/2-F2/2</f>
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="H2">
         <f>A2/2-E2/2</f>
         <v>50</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1280</v>
       </c>
@@ -449,32 +443,29 @@
         <v>720</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C9" si="0">B3/3</f>
+        <f t="shared" ref="C3:C7" si="0">B3/3</f>
         <v>240</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D9" si="1">2*B3/3</f>
+        <f t="shared" ref="D3:D7" si="1">2*B3/3</f>
         <v>480</v>
       </c>
       <c r="E3" s="1">
         <v>620</v>
       </c>
       <c r="F3" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G6" si="2">B3/2-F3/2</f>
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H6" si="3">A3/2-E3/2</f>
         <v>330</v>
       </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>768</v>
       </c>
@@ -493,21 +484,18 @@
         <v>620</v>
       </c>
       <c r="F4" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="2"/>
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1280</v>
       </c>
@@ -526,21 +514,18 @@
         <v>620</v>
       </c>
       <c r="F5" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
         <v>330</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>720</v>
       </c>
@@ -559,21 +544,18 @@
         <v>620</v>
       </c>
       <c r="F6" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="2"/>
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1920</v>
       </c>
@@ -592,87 +574,34 @@
         <v>620</v>
       </c>
       <c r="F7" s="1">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:G9" si="4">B7/2-F7/2</f>
-        <v>300</v>
+        <f t="shared" ref="G7" si="4">B7/2-F7/2</f>
+        <v>283</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H9" si="5">A7/2-E7/2</f>
+        <f t="shared" ref="H7" si="5">A7/2-E7/2</f>
         <v>650</v>
       </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1024</v>
-      </c>
-      <c r="B8" s="1">
-        <v>600</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="E8" s="1">
-        <v>436</v>
-      </c>
-      <c r="F8" s="1">
-        <v>412</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="4"/>
-        <v>94</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="5"/>
-        <v>294</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>600</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1024</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>341.33333333333331</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>682.66666666666663</v>
-      </c>
-      <c r="E9" s="1">
-        <v>436</v>
-      </c>
-      <c r="F9" s="1">
-        <v>412</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="4"/>
-        <v>306</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="5"/>
-        <v>82</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -680,7 +609,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -688,7 +617,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -696,7 +625,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -704,7 +633,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -712,7 +641,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -720,7 +649,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -768,22 +697,6 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for Z3 and Passport
</commit_message>
<xml_diff>
--- a/Image dimensions.xlsx
+++ b/Image dimensions.xlsx
@@ -369,7 +369,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,11 +443,11 @@
         <v>720</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C7" si="0">B3/3</f>
+        <f t="shared" ref="C3:C9" si="0">B3/3</f>
         <v>240</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="1">2*B3/3</f>
+        <f t="shared" ref="D3:D9" si="1">2*B3/3</f>
         <v>480</v>
       </c>
       <c r="E3" s="1">
@@ -577,29 +577,73 @@
         <v>620</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7" si="4">B7/2-F7/2</f>
+        <f t="shared" ref="G7:G9" si="4">B7/2-F7/2</f>
         <v>283</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7" si="5">A7/2-E7/2</f>
+        <f t="shared" ref="H7:H9" si="5">A7/2-E7/2</f>
         <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="1">
+        <v>1440</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1440</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+      <c r="E8" s="1">
+        <v>620</v>
+      </c>
+      <c r="F8" s="1">
+        <v>620</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="4"/>
+        <v>410</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>410</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="1">
+        <v>540</v>
+      </c>
+      <c r="B9" s="1">
+        <v>960</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+      <c r="E9" s="1">
+        <v>420</v>
+      </c>
+      <c r="F9" s="1">
+        <v>420</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>